<commit_message>
Add central data to database setup
</commit_message>
<xml_diff>
--- a/Toilet location dataset.xlsx
+++ b/Toilet location dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6494a95ae17fe58b/Desktop/SC2006 - Software Engineering/SC2006-LooLah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{83B60145-CD85-43E6-9954-C4E554A5A9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E166FDB-4F8F-47B2-AE51-7EEF79520456}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{83B60145-CD85-43E6-9954-C4E554A5A9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0179C464-1091-46AE-9F11-6FDD21D331C9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{323EAB5C-688C-439B-A0FC-FD59FCC086A5}"/>
   </bookViews>
@@ -2252,6 +2252,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2555,7 +2559,7 @@
   <dimension ref="A1:G349"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4436,7 +4440,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>247</v>
       </c>

</xml_diff>